<commit_message>
Update as of March 18, 2025 at 4:45 PM
</commit_message>
<xml_diff>
--- a/res/excel/loadplan_template/load_plan_template.xlsx
+++ b/res/excel/loadplan_template/load_plan_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angeline Labaniego\IdeaProjects\WLP_Automation-v5\res\excel\loadplan_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldri\OneDrive\Desktop\Nikka System\WLP_Automation-v7\res\excel\loadplan_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB18A8AA-5D6D-443F-BA56-A5C9BF5FDCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D68677-335B-4A16-9C0B-123C817A151F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E31B4C9E-2B2E-4045-962C-05F8A6B83FCC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E31B4C9E-2B2E-4045-962C-05F8A6B83FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Plan" sheetId="1" r:id="rId1"/>
@@ -857,34 +857,7 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -929,59 +902,86 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1348,137 +1348,137 @@
   </sheetPr>
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="2" customWidth="1"/>
-    <col min="7" max="14" width="6.75" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.875" style="2"/>
+    <col min="4" max="4" width="8.69921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
+    <col min="7" max="14" width="6.69921875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="6.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.8984375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="G1" s="73" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="G1" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="78" t="s">
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="78"/>
-      <c r="L1" s="71" t="s">
+      <c r="K1" s="69"/>
+      <c r="L1" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="75" t="s">
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="70" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="79" t="s">
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="72" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1493,137 +1493,137 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+    <row r="7" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="80" t="s">
+      <c r="F7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="81" t="s">
+      <c r="M7" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="81"/>
+      <c r="N7" s="72"/>
       <c r="O7" s="18" t="s">
         <v>21</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69" t="s">
+    <row r="8" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="69"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="69"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-    </row>
-    <row r="11" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="82" t="s">
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="60"/>
+    </row>
+    <row r="11" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="66" t="s">
+      <c r="G11" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="62" t="s">
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="P11" s="62" t="s">
+      <c r="P11" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="Q11" s="62" t="s">
+      <c r="Q11" s="59" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="82"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="64"/>
+    <row r="12" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="73"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="78"/>
       <c r="G12" s="44" t="s">
         <v>27</v>
       </c>
@@ -1648,17 +1648,17 @@
       <c r="N12" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="62"/>
-    </row>
-    <row r="13" spans="1:17" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="82"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="65"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+    </row>
+    <row r="13" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A13" s="73"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="79"/>
       <c r="G13" s="45" t="s">
         <v>72</v>
       </c>
@@ -1683,11 +1683,11 @@
       <c r="N13" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="62"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1708,6 +1708,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:N11"/>
     <mergeCell ref="P11:P13"/>
     <mergeCell ref="Q11:Q13"/>
     <mergeCell ref="A8:Q10"/>
@@ -1724,17 +1731,10 @@
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:N11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="153" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="153" scale="98" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -1743,25 +1743,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F57B99B-51F3-4BAF-90D5-6F232EC3A8AD}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24:O31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2"/>
-    <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="2" customWidth="1"/>
-    <col min="7" max="16" width="6.875" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="2"/>
+    <col min="2" max="2" width="10.8984375" style="2"/>
+    <col min="3" max="3" width="12.19921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.8984375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" style="2" customWidth="1"/>
+    <col min="7" max="16" width="6.8984375" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="10.8984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
@@ -1785,7 +1788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>29</v>
       </c>
@@ -1801,7 +1804,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1815,7 +1818,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1829,7 +1832,7 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
     </row>
-    <row r="5" spans="1:15" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="29" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="30" t="s">
         <v>30</v>
       </c>
@@ -1842,7 +1845,7 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
@@ -1856,7 +1859,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1868,14 +1871,14 @@
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="100"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="23" t="s">
         <v>15</v>
       </c>
@@ -1886,12 +1889,12 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="83"/>
+      <c r="D9" s="84"/>
       <c r="E9" s="24"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -1900,7 +1903,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
@@ -1908,19 +1911,19 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="88"/>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="86"/>
       <c r="B11" s="22"/>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="100"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="88"/>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="86"/>
       <c r="B12" s="12"/>
       <c r="C12" s="85" t="s">
         <v>67</v>
@@ -1928,16 +1931,16 @@
       <c r="D12" s="85"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="88"/>
-    </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="86"/>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="100" t="s">
+      <c r="C14" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="100"/>
+      <c r="D14" s="83"/>
       <c r="E14" s="23" t="s">
         <v>15</v>
       </c>
@@ -1948,100 +1951,100 @@
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="C15" s="83" t="s">
+      <c r="C15" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="83"/>
+      <c r="D15" s="84"/>
       <c r="E15" s="24"/>
       <c r="O15" s="22"/>
     </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="G16" s="84" t="s">
+      <c r="G16" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="100" t="s">
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="100"/>
-      <c r="L16" s="100"/>
-      <c r="M16" s="84" t="s">
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
+      <c r="M16" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="84"/>
-      <c r="O16" s="84"/>
-    </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N16" s="87"/>
+      <c r="O16" s="87"/>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="100" t="s">
+      <c r="C17" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="100"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="83" t="s">
+      <c r="J17" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="84"/>
+      <c r="L17" s="84"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="C18" s="83" t="s">
+      <c r="C18" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="83"/>
+      <c r="D18" s="84"/>
       <c r="O18" s="22"/>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="G19" s="84" t="s">
+      <c r="G19" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="100" t="s">
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="100"/>
-      <c r="L19" s="100"/>
-      <c r="M19" s="84" t="s">
+      <c r="K19" s="83"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="N19" s="84"/>
-      <c r="O19" s="84"/>
-    </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N19" s="87"/>
+      <c r="O19" s="87"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="100"/>
+      <c r="D20" s="83"/>
       <c r="E20" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="83" t="s">
+      <c r="J20" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-    </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="84"/>
+      <c r="L20" s="84"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="C21" s="85" t="s">
         <v>65</v>
       </c>
       <c r="D21" s="85"/>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
@@ -2049,21 +2052,21 @@
       <c r="J22" s="21"/>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="84" t="s">
+      <c r="M22" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="N22" s="84"/>
-      <c r="O22" s="84"/>
-    </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N22" s="87"/>
+      <c r="O22" s="87"/>
+    </row>
+    <row r="23" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="100" t="s">
+      <c r="C23" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="100"/>
+      <c r="D23" s="83"/>
       <c r="E23" s="23" t="s">
         <v>15</v>
       </c>
@@ -2074,7 +2077,7 @@
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="C24" s="26" t="s">
         <v>47</v>
@@ -2086,13 +2089,13 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
-      <c r="M24" s="90" t="s">
+      <c r="M24" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="N24" s="91"/>
-      <c r="O24" s="92"/>
-    </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N24" s="90"/>
+      <c r="O24" s="91"/>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
@@ -2100,63 +2103,63 @@
       <c r="J25" s="21"/>
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
-      <c r="M25" s="93"/>
-      <c r="N25" s="94"/>
-      <c r="O25" s="95"/>
-    </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M26" s="93"/>
-      <c r="N26" s="94"/>
-      <c r="O26" s="95"/>
-    </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="84" t="s">
+      <c r="M25" s="92"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="94"/>
+    </row>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M26" s="92"/>
+      <c r="N26" s="93"/>
+      <c r="O26" s="94"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="84"/>
+      <c r="C27" s="87"/>
       <c r="E27" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="89" t="s">
+      <c r="H27" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="I27" s="89"/>
+      <c r="I27" s="88"/>
       <c r="L27" s="32"/>
-      <c r="M27" s="93"/>
-      <c r="N27" s="94"/>
-      <c r="O27" s="95"/>
-    </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M27" s="92"/>
+      <c r="N27" s="93"/>
+      <c r="O27" s="94"/>
+    </row>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="35"/>
       <c r="F28" s="35"/>
       <c r="L28" s="33"/>
-      <c r="M28" s="93"/>
-      <c r="N28" s="94"/>
-      <c r="O28" s="95"/>
-    </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="87" t="s">
+      <c r="M28" s="92"/>
+      <c r="N28" s="93"/>
+      <c r="O28" s="94"/>
+    </row>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87" t="s">
+      <c r="C29" s="98"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87" t="s">
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="98"/>
+      <c r="K29" s="98"/>
       <c r="L29" s="33"/>
-      <c r="M29" s="93"/>
-      <c r="N29" s="94"/>
-      <c r="O29" s="95"/>
-    </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M29" s="92"/>
+      <c r="N29" s="93"/>
+      <c r="O29" s="94"/>
+    </row>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="99" t="s">
         <v>56</v>
       </c>
@@ -2174,46 +2177,45 @@
       <c r="J30" s="99"/>
       <c r="K30" s="99"/>
       <c r="L30" s="34"/>
-      <c r="M30" s="93"/>
-      <c r="N30" s="94"/>
-      <c r="O30" s="95"/>
-    </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="86" t="s">
+      <c r="M30" s="92"/>
+      <c r="N30" s="93"/>
+      <c r="O30" s="94"/>
+    </row>
+    <row r="31" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86" t="s">
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="86" t="s">
+      <c r="F31" s="100"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="100"/>
       <c r="L31" s="23"/>
-      <c r="M31" s="96"/>
-      <c r="N31" s="97"/>
-      <c r="O31" s="98"/>
-    </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="24.6" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="M31" s="95"/>
+      <c r="N31" s="96"/>
+      <c r="O31" s="97"/>
+    </row>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="24.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E29:G29"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="M22:O22"/>
     <mergeCell ref="G16:I16"/>
@@ -2230,17 +2232,18 @@
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="J16:L16"/>
     <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="10000" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="153" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2251,130 +2254,130 @@
   </sheetPr>
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="6.75" style="2" customWidth="1"/>
-    <col min="11" max="12" width="8.625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.75" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="10.875" style="2"/>
+    <col min="4" max="4" width="8.69921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.69921875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="6.69921875" style="2" customWidth="1"/>
+    <col min="11" max="12" width="8.59765625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.69921875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.59765625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="10.8984375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="G1" s="73" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="G1" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="78" t="s">
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="78"/>
-      <c r="L1" s="71" t="s">
+      <c r="K1" s="69"/>
+      <c r="L1" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="75" t="s">
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="70" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="79" t="s">
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="72" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="54" t="s">
         <v>73</v>
       </c>
@@ -2389,10 +2392,10 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+    <row r="7" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="19" t="s">
         <v>16</v>
       </c>
@@ -2413,60 +2416,60 @@
       <c r="N7" s="56"/>
       <c r="O7"/>
     </row>
-    <row r="8" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69" t="s">
+    <row r="8" spans="1:15" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="69"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-    </row>
-    <row r="11" spans="1:15" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+    </row>
+    <row r="11" spans="1:15" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>9</v>
       </c>
@@ -2497,19 +2500,19 @@
       <c r="J11" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="L11" s="68"/>
-      <c r="M11" s="66" t="s">
+      <c r="L11" s="82"/>
+      <c r="M11" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="N11" s="68"/>
+      <c r="N11" s="82"/>
       <c r="O11" s="51" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2528,6 +2531,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
     <mergeCell ref="B6:D7"/>
     <mergeCell ref="A8:O10"/>
     <mergeCell ref="A1:C1"/>
@@ -2539,16 +2548,10 @@
     <mergeCell ref="M2:O3"/>
     <mergeCell ref="D4:L5"/>
     <mergeCell ref="M4:O5"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="10000" scale="93" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="153" scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>